<commit_message>
added Code and MenuDoc
Added to code:
Encoder setup and reading
first few menu screens
battery and arm measurements
change of flame on time and antenna boost,
</commit_message>
<xml_diff>
--- a/INA addresser.xlsx
+++ b/INA addresser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander Nielsen\Desktop\ \hobby\Elektronik\AudioBoxAddOn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F300B742-DE4F-4102-B00B-9DD0C5A76623}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE27201B-FBB3-4358-A7A3-CDAFDA73F790}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{31AE7BDA-4FAC-406A-8BE9-0FE3FA703280}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
   <si>
     <t>A1</t>
   </si>
@@ -58,6 +58,48 @@
   </si>
   <si>
     <t>INA nr</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>HEX add</t>
+  </si>
+  <si>
+    <t>0x4A</t>
+  </si>
+  <si>
+    <t>0x4F</t>
+  </si>
+  <si>
+    <t>testet?</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>0x49</t>
+  </si>
+  <si>
+    <t>0x4E</t>
+  </si>
+  <si>
+    <t>0x46</t>
+  </si>
+  <si>
+    <t>0x4B</t>
+  </si>
+  <si>
+    <t>0x45</t>
+  </si>
+  <si>
+    <t>0x48</t>
+  </si>
+  <si>
+    <t>Grøn</t>
+  </si>
+  <si>
+    <t>orange</t>
   </si>
 </sst>
 </file>
@@ -409,15 +451,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2BCAFB-38DF-4049-8EDA-17A21A2236C1}">
-  <dimension ref="D3:H19"/>
+  <dimension ref="D3:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -433,8 +475,23 @@
       <c r="H3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>5</v>
       </c>
@@ -448,8 +505,23 @@
         <f>BIN2HEX(F4)</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>5</v>
       </c>
@@ -460,11 +532,26 @@
         <v>1000001</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" ref="G5:G19" si="0">BIN2HEX(F5)</f>
+        <f t="shared" ref="G5:G20" si="0">BIN2HEX(F5)</f>
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>5</v>
       </c>
@@ -478,8 +565,23 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -493,8 +595,23 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -508,8 +625,23 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>2</v>
       </c>
@@ -526,8 +658,23 @@
       <c r="H9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>2</v>
       </c>
@@ -544,8 +691,20 @@
       <c r="H10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>2</v>
       </c>
@@ -559,8 +718,23 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>8</v>
+      </c>
+      <c r="L11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>3</v>
       </c>
@@ -578,7 +752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>3</v>
       </c>
@@ -595,8 +769,14 @@
       <c r="H13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>3</v>
       </c>
@@ -614,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>3</v>
       </c>
@@ -632,7 +812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>4</v>
       </c>

</xml_diff>